<commit_message>
arreglando la funcionalidad de iniciar sesion
</commit_message>
<xml_diff>
--- a/app/Plantillas.json/Entrada/eje3.xlsx
+++ b/app/Plantillas.json/Entrada/eje3.xlsx
@@ -758,13 +758,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4367E106-81ED-4E5A-9339-903B282812B4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8424A16-9570-4340-ABE7-532D292049BE}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF9903BD-50E5-45F3-B9F0-0A553016FFBD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB7961BD-6AB2-4AF3-A055-BED07B046BDE}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F708E20F-54CD-4C3A-9168-8ADDD7EC5F81}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{856CE47F-49BC-489F-988E-599C43192D45}"/>
 </file>
</xml_diff>